<commit_message>
fuzzy comfort working -pre library
</commit_message>
<xml_diff>
--- a/Docs/RulesFuzzy.xlsx
+++ b/Docs/RulesFuzzy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Exo-sensing\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C992A89-B7F8-4464-9E70-D76E14DF3C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C122580E-0F0B-4252-9ABD-C4E8D48A329F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{040D37CD-B387-4CC2-B892-E03864DC78EC}"/>
   </bookViews>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4959A959-1C47-4E3A-A881-8AE0EF377B75}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>